<commit_message>
updated Union County Taxes Source Excel Sheet
</commit_message>
<xml_diff>
--- a/2021-2022 Tax Rates/USE THIS FOR - Union County Tax and Fire Rates.xlsx
+++ b/2021-2022 Tax Rates/USE THIS FOR - Union County Tax and Fire Rates.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Current\Tax Matrix\2021-2022 Tax Rates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Current\Tax Matrix\2021-2022 Tax Rates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17295" windowHeight="17760" activeTab="1"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="17295" windowHeight="17760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2021-2022" sheetId="21" r:id="rId1"/>
@@ -1222,15 +1222,6 @@
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1242,6 +1233,15 @@
     </xf>
     <xf numFmtId="167" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2939,19 +2939,19 @@
       <c r="B3" s="107"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="120" t="s">
+      <c r="B5" s="124" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="D13" s="110"/>
       <c r="F13" s="111"/>
-      <c r="H13" s="122">
+      <c r="H13" s="119">
         <v>0.06</v>
       </c>
       <c r="K13" s="109">
@@ -3314,24 +3314,24 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
-      <c r="B41" s="121" t="s">
+      <c r="B41" s="125" t="s">
         <v>137</v>
       </c>
-      <c r="C41" s="121"/>
-      <c r="D41" s="121"/>
+      <c r="C41" s="125"/>
+      <c r="D41" s="125"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="120" t="s">
+      <c r="B42" s="124" t="s">
         <v>145</v>
       </c>
-      <c r="C42" s="120"/>
-      <c r="D42" s="120"/>
+      <c r="C42" s="124"/>
+      <c r="D42" s="124"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="120"/>
-      <c r="C43" s="120"/>
-      <c r="D43" s="120"/>
+      <c r="B43" s="124"/>
+      <c r="C43" s="124"/>
+      <c r="D43" s="124"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
@@ -3639,7 +3639,7 @@
       <c r="A78" s="88" t="s">
         <v>130</v>
       </c>
-      <c r="B78" s="123">
+      <c r="B78" s="120">
         <v>4.0300000000000002E-2</v>
       </c>
       <c r="D78" s="113" t="s">
@@ -10643,8 +10643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" activeCellId="6" sqref="B79 B22 B14 B13 B12 B11 B10"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10671,19 +10671,19 @@
       <c r="B3" s="107"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="120" t="s">
+      <c r="B5" s="124" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
@@ -10715,7 +10715,7 @@
       <c r="A10" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="124">
+      <c r="B10" s="121">
         <v>0.21629999999999999</v>
       </c>
       <c r="D10" s="102" t="s">
@@ -10727,7 +10727,7 @@
       <c r="A11" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="124">
+      <c r="B11" s="121">
         <v>1.5599999999999999E-2</v>
       </c>
       <c r="D11" s="103" t="s">
@@ -10738,7 +10738,7 @@
       <c r="A12" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="124">
+      <c r="B12" s="121">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="D12" s="103" t="s">
@@ -10749,7 +10749,7 @@
       <c r="A13" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="124">
+      <c r="B13" s="121">
         <v>0.44500000000000001</v>
       </c>
       <c r="D13" s="110">
@@ -10760,7 +10760,7 @@
       <c r="A14" s="88" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="124">
+      <c r="B14" s="121">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="D14" s="103" t="s">
@@ -10847,7 +10847,7 @@
       <c r="A22" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="124">
+      <c r="B22" s="121">
         <v>0.38500000000000001</v>
       </c>
       <c r="C22" s="112"/>
@@ -11015,24 +11015,24 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
-      <c r="B42" s="121" t="s">
+      <c r="B42" s="125" t="s">
         <v>137</v>
       </c>
-      <c r="C42" s="121"/>
-      <c r="D42" s="121"/>
+      <c r="C42" s="125"/>
+      <c r="D42" s="125"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="120" t="s">
+      <c r="B43" s="124" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="120"/>
-      <c r="D43" s="120"/>
+      <c r="C43" s="124"/>
+      <c r="D43" s="124"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
-      <c r="B44" s="120"/>
-      <c r="C44" s="120"/>
-      <c r="D44" s="120"/>
+      <c r="B44" s="124"/>
+      <c r="C44" s="124"/>
+      <c r="D44" s="124"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
@@ -11173,7 +11173,7 @@
         <v>112</v>
       </c>
       <c r="B61" s="104">
-        <v>5.3100000000000001E-2</v>
+        <v>3.3500000000000002E-2</v>
       </c>
       <c r="D61" s="113" t="s">
         <v>113</v>
@@ -11340,7 +11340,7 @@
       <c r="A79" s="88" t="s">
         <v>130</v>
       </c>
-      <c r="B79" s="125">
+      <c r="B79" s="122">
         <v>5.2600000000000001E-2</v>
       </c>
       <c r="D79" s="113" t="s">

</xml_diff>

<commit_message>
updated union xslx file
</commit_message>
<xml_diff>
--- a/2021-2022 Tax Rates/USE THIS FOR - Union County Tax and Fire Rates.xlsx
+++ b/2021-2022 Tax Rates/USE THIS FOR - Union County Tax and Fire Rates.xlsx
@@ -5,38 +5,39 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Current\Tax Matrix\2021-2022 Tax Rates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\gig\local_repos\base_tax-matrix\2021-2022 Tax Rates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="17295" windowHeight="17760" activeTab="1"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="17295" windowHeight="17760"/>
   </bookViews>
   <sheets>
-    <sheet name="2021-2022" sheetId="21" r:id="rId1"/>
-    <sheet name="2020-2021" sheetId="20" r:id="rId2"/>
-    <sheet name="2019-2020" sheetId="19" r:id="rId3"/>
-    <sheet name="2018-2019" sheetId="17" r:id="rId4"/>
-    <sheet name="2017-2018" sheetId="15" r:id="rId5"/>
-    <sheet name="2016-2017" sheetId="14" r:id="rId6"/>
-    <sheet name="2015-2016" sheetId="12" r:id="rId7"/>
-    <sheet name="2014-2015" sheetId="13" r:id="rId8"/>
-    <sheet name="2013 - 2014" sheetId="10" r:id="rId9"/>
-    <sheet name="2012 - 2013" sheetId="7" r:id="rId10"/>
-    <sheet name="2011-2012" sheetId="8" r:id="rId11"/>
-    <sheet name="2010 - 2011" sheetId="6" r:id="rId12"/>
-    <sheet name="2009-2010" sheetId="5" r:id="rId13"/>
-    <sheet name="2008-2009" sheetId="9" r:id="rId14"/>
-    <sheet name="2007-2008" sheetId="4" r:id="rId15"/>
-    <sheet name="2006-2007" sheetId="3" r:id="rId16"/>
-    <sheet name="2005-2006" sheetId="1" r:id="rId17"/>
-    <sheet name="Prior Year Tax Rates" sheetId="11" r:id="rId18"/>
+    <sheet name="2022-2023" sheetId="22" r:id="rId1"/>
+    <sheet name="2021-2022" sheetId="21" r:id="rId2"/>
+    <sheet name="2020-2021" sheetId="20" r:id="rId3"/>
+    <sheet name="2019-2020" sheetId="19" r:id="rId4"/>
+    <sheet name="2018-2019" sheetId="17" r:id="rId5"/>
+    <sheet name="2017-2018" sheetId="15" r:id="rId6"/>
+    <sheet name="2016-2017" sheetId="14" r:id="rId7"/>
+    <sheet name="2015-2016" sheetId="12" r:id="rId8"/>
+    <sheet name="2014-2015" sheetId="13" r:id="rId9"/>
+    <sheet name="2013 - 2014" sheetId="10" r:id="rId10"/>
+    <sheet name="2012 - 2013" sheetId="7" r:id="rId11"/>
+    <sheet name="2011-2012" sheetId="8" r:id="rId12"/>
+    <sheet name="2010 - 2011" sheetId="6" r:id="rId13"/>
+    <sheet name="2009-2010" sheetId="5" r:id="rId14"/>
+    <sheet name="2008-2009" sheetId="9" r:id="rId15"/>
+    <sheet name="2007-2008" sheetId="4" r:id="rId16"/>
+    <sheet name="2006-2007" sheetId="3" r:id="rId17"/>
+    <sheet name="2005-2006" sheetId="1" r:id="rId18"/>
+    <sheet name="Prior Year Tax Rates" sheetId="11" r:id="rId19"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="146">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1277,7 +1278,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1315,7 +1316,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1342,6 +1343,79 @@
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1543050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9275" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="352425" y="114300"/>
+          <a:ext cx="1190625" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1414,7 +1488,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1487,7 +1561,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1560,7 +1634,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1633,7 +1707,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1706,7 +1780,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1779,7 +1853,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1852,7 +1926,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1926,6 +2000,87 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1618235</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>230266</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="142875" y="8791575"/>
+          <a:ext cx="1475360" cy="1678066"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1694435</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1666</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="219075" y="9525"/>
+          <a:ext cx="1475360" cy="1639966"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2006,7 +2161,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2084,7 +2239,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2162,7 +2317,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2240,7 +2395,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2318,7 +2473,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2391,7 +2546,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2430,79 +2585,6 @@
         <a:xfrm>
           <a:off x="352425" y="114300"/>
           <a:ext cx="876300" cy="1104900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1543050</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9275" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="352425" y="114300"/>
-          <a:ext cx="1190625" cy="1104900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2911,8 +2993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3701,6 +3783,438 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:IV65536"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="31" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="C5" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="D10" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="38">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="37"/>
+      <c r="B12" s="38"/>
+    </row>
+    <row r="13" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="38">
+        <v>0</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="37"/>
+      <c r="B14" s="38"/>
+    </row>
+    <row r="15" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="38">
+        <v>0.05</v>
+      </c>
+      <c r="D15" s="39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="37"/>
+      <c r="B16" s="38"/>
+    </row>
+    <row r="17" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="38">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="D17" s="39">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+    </row>
+    <row r="19" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="38">
+        <v>0.2</v>
+      </c>
+      <c r="D19" s="39">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="37"/>
+      <c r="B20" s="38"/>
+    </row>
+    <row r="21" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="38">
+        <v>0.39</v>
+      </c>
+      <c r="D21" s="39">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="37"/>
+      <c r="B22" s="38"/>
+    </row>
+    <row r="23" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="38">
+        <v>0.48</v>
+      </c>
+      <c r="C23" s="41"/>
+      <c r="D23" s="39">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="37"/>
+      <c r="B24" s="38"/>
+    </row>
+    <row r="25" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="38">
+        <v>0.34</v>
+      </c>
+      <c r="C25" s="40"/>
+      <c r="D25" s="39">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="37"/>
+      <c r="B26" s="38"/>
+    </row>
+    <row r="27" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="38">
+        <v>0.185</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="39">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="39" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="37"/>
+      <c r="B28" s="38"/>
+    </row>
+    <row r="29" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="42">
+        <v>0.215</v>
+      </c>
+      <c r="D29" s="39">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="39" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="37"/>
+      <c r="B30" s="38"/>
+    </row>
+    <row r="31" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="43">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="D31" s="39">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="37"/>
+      <c r="B32" s="38"/>
+    </row>
+    <row r="33" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="38">
+        <v>0.23</v>
+      </c>
+      <c r="D33" s="39">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="38"/>
+    </row>
+    <row r="35" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="D35" s="39">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="37"/>
+      <c r="B36" s="38"/>
+    </row>
+    <row r="37" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="43">
+        <v>0</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="39">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="37"/>
+      <c r="B38" s="38"/>
+    </row>
+    <row r="39" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="38">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="D39" s="39">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="37"/>
+      <c r="B40" s="38"/>
+    </row>
+    <row r="41" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="38">
+        <v>0.02</v>
+      </c>
+      <c r="D41" s="39">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="37"/>
+      <c r="B42" s="38"/>
+    </row>
+    <row r="43" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="38">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D43" s="39">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="37"/>
+      <c r="B44" s="38"/>
+    </row>
+    <row r="45" spans="1:4" s="39" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="43">
+        <v>0</v>
+      </c>
+      <c r="C45" s="44"/>
+      <c r="D45" s="39">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="37"/>
+      <c r="B46" s="38"/>
+    </row>
+    <row r="47" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="38">
+        <v>4.2799999999999998E-2</v>
+      </c>
+      <c r="D47" s="39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="37"/>
+      <c r="B48" s="38"/>
+    </row>
+    <row r="49" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="38">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="D49" s="39">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="37"/>
+      <c r="B50" s="38"/>
+    </row>
+    <row r="51" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" s="38">
+        <v>2.41E-2</v>
+      </c>
+      <c r="D51" s="39">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="37"/>
+      <c r="B52" s="38"/>
+    </row>
+    <row r="53" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B53" s="38">
+        <v>3.8600000000000002E-2</v>
+      </c>
+      <c r="C53" s="41"/>
+      <c r="D53" s="39">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="37"/>
+      <c r="B54" s="38"/>
+    </row>
+    <row r="55" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55" s="38">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="D55" s="39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;CAs of &amp;D REM</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E58"/>
+  <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
@@ -4129,7 +4643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
@@ -4558,7 +5072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
@@ -4989,7 +5503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
@@ -5524,7 +6038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
@@ -5952,7 +6466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
@@ -6390,7 +6904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
@@ -6828,7 +7342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
@@ -7253,7 +7767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X73"/>
   <sheetViews>
@@ -10641,10 +11155,800 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K82"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" style="108" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="108" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="108" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="108" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="108"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="107"/>
+    </row>
+    <row r="2" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="107"/>
+    </row>
+    <row r="3" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="107"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="123" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="124" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="107"/>
+    </row>
+    <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="107"/>
+    </row>
+    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="107"/>
+      <c r="D9" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="88" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" s="104">
+        <v>0.48549999999999999</v>
+      </c>
+      <c r="D10" s="102" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="99"/>
+      <c r="H10" s="109">
+        <v>0.48549999999999999</v>
+      </c>
+      <c r="K10" s="109">
+        <v>0.21629999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="88" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="104">
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="D11" s="103" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="109">
+        <v>0.19</v>
+      </c>
+      <c r="K11" s="109">
+        <v>1.3299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="104">
+        <v>0.06</v>
+      </c>
+      <c r="D12" s="110">
+        <v>100</v>
+      </c>
+      <c r="F12" s="111"/>
+      <c r="H12" s="109">
+        <v>4.41E-2</v>
+      </c>
+      <c r="K12" s="109">
+        <v>2.3300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="117" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" s="116">
+        <v>61</v>
+      </c>
+      <c r="D13" s="110"/>
+      <c r="F13" s="111"/>
+      <c r="H13" s="119">
+        <v>0.06</v>
+      </c>
+      <c r="K13" s="109">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="117" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" s="116"/>
+      <c r="D14" s="110"/>
+      <c r="F14" s="111"/>
+      <c r="K14" s="109">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="88" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="104">
+        <v>0.50249999999999995</v>
+      </c>
+      <c r="D15" s="110">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="117" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="104">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="C16" s="118"/>
+      <c r="D16" s="110"/>
+    </row>
+    <row r="17" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="117" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="116">
+        <v>30</v>
+      </c>
+      <c r="D17" s="110">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="88" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="104">
+        <v>0.34</v>
+      </c>
+      <c r="D18" s="110">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="117" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" s="116">
+        <v>25</v>
+      </c>
+      <c r="D19" s="110"/>
+      <c r="K19" s="109">
+        <v>0.21629999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="88" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="104">
+        <v>0.49</v>
+      </c>
+      <c r="C20" s="97"/>
+      <c r="D20" s="110">
+        <v>400</v>
+      </c>
+      <c r="K20" s="109">
+        <v>1.56E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="88" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="104">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="C21" s="112"/>
+      <c r="D21" s="110">
+        <v>500</v>
+      </c>
+      <c r="K21" s="109">
+        <v>2.0999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="117" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="116">
+        <v>25</v>
+      </c>
+      <c r="D22" s="110"/>
+      <c r="K22" s="109">
+        <v>5.2599999999999999E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="88" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="104">
+        <v>0.185</v>
+      </c>
+      <c r="C23" s="98"/>
+      <c r="D23" s="110">
+        <v>600</v>
+      </c>
+      <c r="K23" s="109">
+        <v>3.3E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="117" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" s="104"/>
+      <c r="C24" s="98"/>
+      <c r="D24" s="110"/>
+    </row>
+    <row r="25" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="104">
+        <v>0.186</v>
+      </c>
+      <c r="D25" s="110">
+        <v>700</v>
+      </c>
+      <c r="K25" s="109">
+        <f>SUM(K19:K24)</f>
+        <v>0.22851999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="117" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26" s="104"/>
+      <c r="D26" s="110"/>
+    </row>
+    <row r="27" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="88" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="104">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="D27" s="110">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="88" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="104">
+        <v>0.19</v>
+      </c>
+      <c r="D28" s="110">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="117" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="104"/>
+      <c r="D29" s="110"/>
+    </row>
+    <row r="30" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="104">
+        <v>0.02</v>
+      </c>
+      <c r="D30" s="110">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="88" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="104">
+        <v>0</v>
+      </c>
+      <c r="C31" s="98"/>
+      <c r="D31" s="110">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="88" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="104">
+        <v>1.29E-2</v>
+      </c>
+      <c r="D32" s="110">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="88" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="104">
+        <v>0.02</v>
+      </c>
+      <c r="D33" s="110">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="109" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="88" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="104">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D34" s="110">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="115" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="114">
+        <v>0</v>
+      </c>
+      <c r="D35" s="110">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="115"/>
+      <c r="B36" s="114"/>
+      <c r="D36" s="110"/>
+    </row>
+    <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="107"/>
+    </row>
+    <row r="40" spans="1:5" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="107"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="125" t="s">
+        <v>137</v>
+      </c>
+      <c r="C41" s="125"/>
+      <c r="D41" s="125"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="124" t="s">
+        <v>145</v>
+      </c>
+      <c r="C42" s="124"/>
+      <c r="D42" s="124"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="124"/>
+      <c r="C43" s="124"/>
+      <c r="D43" s="124"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="107"/>
+    </row>
+    <row r="45" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="107"/>
+    </row>
+    <row r="46" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="107"/>
+      <c r="D47" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="88" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="104">
+        <v>2.1499999999999998E-2</v>
+      </c>
+      <c r="D48" s="113" t="s">
+        <v>102</v>
+      </c>
+      <c r="E48" s="106"/>
+    </row>
+    <row r="49" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="88"/>
+      <c r="B49" s="104"/>
+      <c r="D49" s="113"/>
+      <c r="E49" s="106"/>
+    </row>
+    <row r="50" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="104">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="D50" s="113" t="s">
+        <v>104</v>
+      </c>
+      <c r="E50" s="91"/>
+    </row>
+    <row r="51" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="88"/>
+      <c r="B51" s="104"/>
+      <c r="D51" s="113"/>
+      <c r="E51" s="91"/>
+    </row>
+    <row r="52" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="88" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="104">
+        <v>4.2200000000000001E-2</v>
+      </c>
+      <c r="D52" s="113" t="s">
+        <v>106</v>
+      </c>
+      <c r="E52" s="91"/>
+    </row>
+    <row r="53" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="88"/>
+      <c r="B53" s="104"/>
+      <c r="D53" s="113"/>
+      <c r="E53" s="91"/>
+    </row>
+    <row r="54" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="88" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="104">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D54" s="113" t="s">
+        <v>108</v>
+      </c>
+      <c r="E54" s="91"/>
+    </row>
+    <row r="55" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="88"/>
+      <c r="B55" s="104"/>
+      <c r="D55" s="113"/>
+      <c r="E55" s="91"/>
+    </row>
+    <row r="56" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="88" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="104">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="D56" s="113" t="s">
+        <v>110</v>
+      </c>
+      <c r="E56" s="91"/>
+    </row>
+    <row r="57" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="88"/>
+      <c r="B57" s="104"/>
+      <c r="D57" s="113"/>
+      <c r="E57" s="91"/>
+    </row>
+    <row r="58" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="88" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" s="104">
+        <v>6.4399999999999999E-2</v>
+      </c>
+      <c r="D58" s="113" t="s">
+        <v>111</v>
+      </c>
+      <c r="E58" s="91"/>
+    </row>
+    <row r="59" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="88"/>
+      <c r="B59" s="104"/>
+      <c r="D59" s="113"/>
+      <c r="E59" s="91"/>
+    </row>
+    <row r="60" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="88" t="s">
+        <v>112</v>
+      </c>
+      <c r="B60" s="104">
+        <v>3.3500000000000002E-2</v>
+      </c>
+      <c r="D60" s="113" t="s">
+        <v>113</v>
+      </c>
+      <c r="E60" s="91"/>
+    </row>
+    <row r="61" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="88"/>
+      <c r="B61" s="104"/>
+      <c r="D61" s="113"/>
+      <c r="E61" s="91"/>
+    </row>
+    <row r="62" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="88" t="s">
+        <v>114</v>
+      </c>
+      <c r="B62" s="104">
+        <v>4.7199999999999999E-2</v>
+      </c>
+      <c r="D62" s="113" t="s">
+        <v>115</v>
+      </c>
+      <c r="E62" s="91"/>
+    </row>
+    <row r="63" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="88"/>
+      <c r="B63" s="104"/>
+      <c r="D63" s="113"/>
+      <c r="E63" s="91"/>
+    </row>
+    <row r="64" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="88" t="s">
+        <v>116</v>
+      </c>
+      <c r="B64" s="104">
+        <v>6.1600000000000002E-2</v>
+      </c>
+      <c r="D64" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="E64" s="91"/>
+    </row>
+    <row r="65" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="88"/>
+      <c r="B65" s="104"/>
+      <c r="D65" s="113"/>
+      <c r="E65" s="91"/>
+    </row>
+    <row r="66" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="88" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" s="104">
+        <v>6.6299999999999998E-2</v>
+      </c>
+      <c r="D66" s="113" t="s">
+        <v>119</v>
+      </c>
+      <c r="E66" s="91"/>
+    </row>
+    <row r="67" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="88"/>
+      <c r="B67" s="104"/>
+      <c r="D67" s="113"/>
+      <c r="E67" s="91"/>
+    </row>
+    <row r="68" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="B68" s="104">
+        <v>4.41E-2</v>
+      </c>
+      <c r="D68" s="113" t="s">
+        <v>121</v>
+      </c>
+      <c r="E68" s="91"/>
+    </row>
+    <row r="69" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="88"/>
+      <c r="B69" s="104"/>
+      <c r="D69" s="113"/>
+      <c r="E69" s="91"/>
+    </row>
+    <row r="70" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="88" t="s">
+        <v>122</v>
+      </c>
+      <c r="B70" s="104">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C70" s="97"/>
+      <c r="D70" s="113" t="s">
+        <v>123</v>
+      </c>
+      <c r="E70" s="91"/>
+    </row>
+    <row r="71" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="88"/>
+      <c r="B71" s="104"/>
+      <c r="C71" s="97"/>
+      <c r="D71" s="113"/>
+      <c r="E71" s="91"/>
+    </row>
+    <row r="72" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="B72" s="104">
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="C72" s="112"/>
+      <c r="D72" s="113" t="s">
+        <v>125</v>
+      </c>
+      <c r="E72" s="91"/>
+    </row>
+    <row r="73" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="88"/>
+      <c r="B73" s="104"/>
+      <c r="C73" s="112"/>
+      <c r="D73" s="113"/>
+      <c r="E73" s="91"/>
+    </row>
+    <row r="74" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="88" t="s">
+        <v>126</v>
+      </c>
+      <c r="B74" s="104">
+        <v>3.61E-2</v>
+      </c>
+      <c r="D74" s="113" t="s">
+        <v>127</v>
+      </c>
+      <c r="E74" s="91"/>
+    </row>
+    <row r="75" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="88"/>
+      <c r="B75" s="104"/>
+      <c r="D75" s="113"/>
+      <c r="E75" s="91"/>
+    </row>
+    <row r="76" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="88" t="s">
+        <v>128</v>
+      </c>
+      <c r="B76" s="104">
+        <v>5.6800000000000003E-2</v>
+      </c>
+      <c r="C76" s="98"/>
+      <c r="D76" s="113" t="s">
+        <v>129</v>
+      </c>
+      <c r="E76" s="91"/>
+    </row>
+    <row r="77" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="88"/>
+      <c r="B77" s="104"/>
+      <c r="C77" s="98"/>
+      <c r="D77" s="113"/>
+      <c r="E77" s="91"/>
+    </row>
+    <row r="78" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="88" t="s">
+        <v>130</v>
+      </c>
+      <c r="B78" s="120">
+        <v>4.0300000000000002E-2</v>
+      </c>
+      <c r="D78" s="113" t="s">
+        <v>131</v>
+      </c>
+      <c r="E78" s="91"/>
+    </row>
+    <row r="79" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="88"/>
+      <c r="B79" s="104"/>
+      <c r="D79" s="113"/>
+      <c r="E79" s="91"/>
+    </row>
+    <row r="80" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="88" t="s">
+        <v>132</v>
+      </c>
+      <c r="B80" s="104">
+        <v>3.85E-2</v>
+      </c>
+      <c r="D80" s="113" t="s">
+        <v>133</v>
+      </c>
+      <c r="E80" s="91"/>
+    </row>
+    <row r="81" spans="1:5" s="109" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="88"/>
+      <c r="B81" s="104"/>
+      <c r="D81" s="113"/>
+      <c r="E81" s="91"/>
+    </row>
+    <row r="82" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="88" t="s">
+        <v>134</v>
+      </c>
+      <c r="B82" s="104">
+        <v>3.61E-2</v>
+      </c>
+      <c r="D82" s="113" t="s">
+        <v>135</v>
+      </c>
+      <c r="E82" s="91"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11398,7 +12702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -11812,7 +13116,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F64"/>
   <sheetViews>
@@ -12307,7 +13611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F64"/>
   <sheetViews>
@@ -12802,7 +14106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F62"/>
   <sheetViews>
@@ -13270,7 +14574,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F62"/>
   <sheetViews>
@@ -13741,7 +15045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
@@ -14168,436 +15472,4 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:IV65536"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="31" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="C5" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="D10" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="38">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="37"/>
-      <c r="B12" s="38"/>
-    </row>
-    <row r="13" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="38">
-        <v>0</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="37"/>
-      <c r="B14" s="38"/>
-    </row>
-    <row r="15" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="38">
-        <v>0.05</v>
-      </c>
-      <c r="D15" s="39">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="37"/>
-      <c r="B16" s="38"/>
-    </row>
-    <row r="17" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="38">
-        <v>0.55500000000000005</v>
-      </c>
-      <c r="D17" s="39">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
-      <c r="B18" s="38"/>
-    </row>
-    <row r="19" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="38">
-        <v>0.2</v>
-      </c>
-      <c r="D19" s="39">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
-      <c r="B20" s="38"/>
-    </row>
-    <row r="21" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="38">
-        <v>0.39</v>
-      </c>
-      <c r="D21" s="39">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="37"/>
-      <c r="B22" s="38"/>
-    </row>
-    <row r="23" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="38">
-        <v>0.48</v>
-      </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="39">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="37"/>
-      <c r="B24" s="38"/>
-    </row>
-    <row r="25" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="38">
-        <v>0.34</v>
-      </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="39">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="37"/>
-      <c r="B26" s="38"/>
-    </row>
-    <row r="27" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="38">
-        <v>0.185</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="39">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="39" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="37"/>
-      <c r="B28" s="38"/>
-    </row>
-    <row r="29" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="42">
-        <v>0.215</v>
-      </c>
-      <c r="D29" s="39">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="39" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="37"/>
-      <c r="B30" s="38"/>
-    </row>
-    <row r="31" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="43">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="D31" s="39">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="37"/>
-      <c r="B32" s="38"/>
-    </row>
-    <row r="33" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="38">
-        <v>0.23</v>
-      </c>
-      <c r="D33" s="39">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="38"/>
-    </row>
-    <row r="35" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="38">
-        <v>0.02</v>
-      </c>
-      <c r="D35" s="39">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="37"/>
-      <c r="B36" s="38"/>
-    </row>
-    <row r="37" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37" s="43">
-        <v>0</v>
-      </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="39">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="37"/>
-      <c r="B38" s="38"/>
-    </row>
-    <row r="39" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="38">
-        <v>1.6500000000000001E-2</v>
-      </c>
-      <c r="D39" s="39">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="37"/>
-      <c r="B40" s="38"/>
-    </row>
-    <row r="41" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="B41" s="38">
-        <v>0.02</v>
-      </c>
-      <c r="D41" s="39">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="37"/>
-      <c r="B42" s="38"/>
-    </row>
-    <row r="43" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43" s="38">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D43" s="39">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="37"/>
-      <c r="B44" s="38"/>
-    </row>
-    <row r="45" spans="1:4" s="39" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45" s="43">
-        <v>0</v>
-      </c>
-      <c r="C45" s="44"/>
-      <c r="D45" s="39">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="37"/>
-      <c r="B46" s="38"/>
-    </row>
-    <row r="47" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="38">
-        <v>4.2799999999999998E-2</v>
-      </c>
-      <c r="D47" s="39">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="37"/>
-      <c r="B48" s="38"/>
-    </row>
-    <row r="49" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="B49" s="38">
-        <v>5.2600000000000001E-2</v>
-      </c>
-      <c r="D49" s="39">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="39" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="37"/>
-      <c r="B50" s="38"/>
-    </row>
-    <row r="51" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B51" s="38">
-        <v>2.41E-2</v>
-      </c>
-      <c r="D51" s="39">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" s="39" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="37"/>
-      <c r="B52" s="38"/>
-    </row>
-    <row r="53" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="B53" s="38">
-        <v>3.8600000000000002E-2</v>
-      </c>
-      <c r="C53" s="41"/>
-      <c r="D53" s="39">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="37"/>
-      <c r="B54" s="38"/>
-    </row>
-    <row r="55" spans="1:4" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="B55" s="38">
-        <v>3.5499999999999997E-2</v>
-      </c>
-      <c r="D55" s="39">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="1"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;CAs of &amp;D REM</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>